<commit_message>
新增 .gitignore 檔案以忽略 file_metadata.json，並在 analyze_stock.py 中初始化 metadata 檔案，從 Excel 擷取日期並儲存至 metadata
</commit_message>
<xml_diff>
--- a/未實現損益試算.xlsx
+++ b/未實現損益試算.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\python project\my-stock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD8ACEE3-2569-4D84-9876-E7DB6CCA3BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B752F5D-C044-49EB-A8C7-16873F0C6B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="2240" windowWidth="19200" windowHeight="10060" xr2:uid="{2C999212-4BDB-421B-BBC4-3D898A9695EB}"/>
+    <workbookView xWindow="2240" yWindow="2240" windowWidth="19200" windowHeight="10060" xr2:uid="{F3ECF929-4890-4C97-A22F-A9B5B2393B5F}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -518,7 +518,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6399FA3-4D51-472D-8A19-82C94836BA3D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB4F7F3B-7EFF-4F4F-A6C4-6873FBD66385}">
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -595,28 +595,28 @@
         <v>15</v>
       </c>
       <c r="D2" s="2">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="E2" s="2">
-        <v>43.94</v>
+        <v>44.9</v>
       </c>
       <c r="F2" s="2">
-        <v>7387</v>
+        <v>8851</v>
       </c>
       <c r="G2" s="2">
-        <v>8520</v>
+        <v>9978</v>
       </c>
       <c r="H2" s="2">
-        <v>1133</v>
+        <v>1127</v>
       </c>
       <c r="I2" s="3">
-        <v>0.153</v>
+        <v>0.127</v>
       </c>
       <c r="J2" s="2">
         <v>51</v>
       </c>
       <c r="K2" s="2">
-        <v>8568</v>
+        <v>10047</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>16</v>
@@ -636,25 +636,25 @@
         <v>58</v>
       </c>
       <c r="E3" s="2">
-        <v>53.19</v>
+        <v>49.64</v>
       </c>
       <c r="F3" s="2">
-        <v>3087</v>
+        <v>2881</v>
       </c>
       <c r="G3" s="2">
-        <v>2571</v>
+        <v>2640</v>
       </c>
       <c r="H3" s="2">
-        <v>-516</v>
+        <v>-241</v>
       </c>
       <c r="I3" s="3">
-        <v>-0.16700000000000001</v>
+        <v>-8.4000000000000005E-2</v>
       </c>
       <c r="J3" s="2">
-        <v>44.8</v>
+        <v>46</v>
       </c>
       <c r="K3" s="2">
-        <v>2598</v>
+        <v>2668</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>16</v>
@@ -680,19 +680,19 @@
         <v>5121</v>
       </c>
       <c r="G4" s="2">
-        <v>4583</v>
+        <v>4550</v>
       </c>
       <c r="H4" s="2">
-        <v>-538</v>
+        <v>-571</v>
       </c>
       <c r="I4" s="3">
-        <v>-0.105</v>
+        <v>-0.112</v>
       </c>
       <c r="J4" s="2">
-        <v>140.5</v>
+        <v>139.5</v>
       </c>
       <c r="K4" s="2">
-        <v>4636</v>
+        <v>4604</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>16</v>
@@ -718,19 +718,19 @@
         <v>2883</v>
       </c>
       <c r="G5" s="2">
-        <v>2305</v>
+        <v>2508</v>
       </c>
       <c r="H5" s="2">
-        <v>-578</v>
+        <v>-375</v>
       </c>
       <c r="I5" s="3">
-        <v>-0.2</v>
+        <v>-0.13</v>
       </c>
       <c r="J5" s="2">
-        <v>75.2</v>
+        <v>81.8</v>
       </c>
       <c r="K5" s="2">
-        <v>2331</v>
+        <v>2536</v>
       </c>
       <c r="N5" s="2" t="s">
         <v>16</v>
@@ -756,19 +756,19 @@
         <v>118735</v>
       </c>
       <c r="G6" s="2">
-        <v>136744</v>
+        <v>137942</v>
       </c>
       <c r="H6" s="2">
-        <v>18009</v>
+        <v>19207</v>
       </c>
       <c r="I6" s="3">
-        <v>0.152</v>
+        <v>0.16200000000000001</v>
       </c>
       <c r="J6" s="2">
-        <v>1145</v>
+        <v>1155</v>
       </c>
       <c r="K6" s="2">
-        <v>137400</v>
+        <v>138600</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>16</v>
@@ -794,19 +794,19 @@
         <v>3186</v>
       </c>
       <c r="G7" s="2">
-        <v>3825</v>
+        <v>4008</v>
       </c>
       <c r="H7" s="2">
-        <v>639</v>
+        <v>822</v>
       </c>
       <c r="I7" s="3">
-        <v>0.20100000000000001</v>
+        <v>0.25800000000000001</v>
       </c>
       <c r="J7" s="2">
-        <v>96.4</v>
+        <v>101</v>
       </c>
       <c r="K7" s="2">
-        <v>3856</v>
+        <v>4040</v>
       </c>
       <c r="N7" s="2" t="s">
         <v>16</v>
@@ -832,19 +832,19 @@
         <v>198650</v>
       </c>
       <c r="G8" s="2">
-        <v>239499</v>
+        <v>242767</v>
       </c>
       <c r="H8" s="2">
-        <v>40849</v>
+        <v>44117</v>
       </c>
       <c r="I8" s="3">
-        <v>0.20599999999999999</v>
+        <v>0.222</v>
       </c>
       <c r="J8" s="2">
-        <v>65.900000000000006</v>
+        <v>66.8</v>
       </c>
       <c r="K8" s="2">
-        <v>240667</v>
+        <v>243954</v>
       </c>
       <c r="N8" s="2" t="s">
         <v>16</v>
@@ -870,19 +870,19 @@
         <v>60493</v>
       </c>
       <c r="G9" s="2">
-        <v>51516</v>
+        <v>51975</v>
       </c>
       <c r="H9" s="2">
-        <v>-8977</v>
+        <v>-8518</v>
       </c>
       <c r="I9" s="3">
-        <v>-0.14799999999999999</v>
+        <v>-0.14099999999999999</v>
       </c>
       <c r="J9" s="2">
-        <v>78.5</v>
+        <v>79.2</v>
       </c>
       <c r="K9" s="2">
-        <v>51888</v>
+        <v>52351</v>
       </c>
       <c r="N9" s="2" t="s">
         <v>16</v>
@@ -908,19 +908,19 @@
         <v>2959</v>
       </c>
       <c r="G10" s="2">
-        <v>2698</v>
+        <v>2676</v>
       </c>
       <c r="H10" s="2">
-        <v>-261</v>
+        <v>-283</v>
       </c>
       <c r="I10" s="3">
-        <v>-8.7999999999999995E-2</v>
+        <v>-9.6000000000000002E-2</v>
       </c>
       <c r="J10" s="2">
-        <v>41.95</v>
+        <v>41.6</v>
       </c>
       <c r="K10" s="2">
-        <v>2727</v>
+        <v>2704</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>16</v>
@@ -946,19 +946,19 @@
         <v>42026</v>
       </c>
       <c r="G11" s="2">
-        <v>40368</v>
+        <v>39837</v>
       </c>
       <c r="H11" s="2">
-        <v>-1658</v>
+        <v>-2189</v>
       </c>
       <c r="I11" s="3">
-        <v>-3.9E-2</v>
+        <v>-5.1999999999999998E-2</v>
       </c>
       <c r="J11" s="2">
-        <v>83.6</v>
+        <v>82.5</v>
       </c>
       <c r="K11" s="2">
-        <v>40546</v>
+        <v>40012</v>
       </c>
       <c r="N11" s="2" t="s">
         <v>16</v>
@@ -984,19 +984,19 @@
         <v>29006</v>
       </c>
       <c r="G12" s="2">
-        <v>30142</v>
+        <v>29718</v>
       </c>
       <c r="H12" s="2">
-        <v>1136</v>
+        <v>712</v>
       </c>
       <c r="I12" s="3">
-        <v>3.9E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="J12" s="2">
-        <v>32.049999999999997</v>
+        <v>31.6</v>
       </c>
       <c r="K12" s="2">
-        <v>30287</v>
+        <v>29862</v>
       </c>
       <c r="N12" s="2" t="s">
         <v>16</v>
@@ -1022,19 +1022,19 @@
         <v>6067</v>
       </c>
       <c r="G13" s="2">
-        <v>5864</v>
+        <v>5850</v>
       </c>
       <c r="H13" s="2">
-        <v>-203</v>
+        <v>-217</v>
       </c>
       <c r="I13" s="3">
-        <v>-3.3000000000000002E-2</v>
+        <v>-3.5999999999999997E-2</v>
       </c>
       <c r="J13" s="2">
-        <v>84.3</v>
+        <v>84.1</v>
       </c>
       <c r="K13" s="2">
-        <v>5901</v>
+        <v>5887</v>
       </c>
       <c r="N13" s="2" t="s">
         <v>16</v>
@@ -1060,19 +1060,19 @@
         <v>5328</v>
       </c>
       <c r="G14" s="2">
-        <v>6737</v>
+        <v>6702</v>
       </c>
       <c r="H14" s="2">
-        <v>1409</v>
+        <v>1374</v>
       </c>
       <c r="I14" s="3">
-        <v>0.26400000000000001</v>
+        <v>0.25800000000000001</v>
       </c>
       <c r="J14" s="2">
-        <v>37.15</v>
+        <v>36.950000000000003</v>
       </c>
       <c r="K14" s="2">
-        <v>6798</v>
+        <v>6762</v>
       </c>
       <c r="N14" s="2" t="s">
         <v>16</v>
@@ -1098,19 +1098,19 @@
         <v>3033</v>
       </c>
       <c r="G15" s="2">
-        <v>2161</v>
+        <v>2191</v>
       </c>
       <c r="H15" s="2">
-        <v>-872</v>
+        <v>-842</v>
       </c>
       <c r="I15" s="3">
-        <v>-0.28799999999999998</v>
+        <v>-0.27800000000000002</v>
       </c>
       <c r="J15" s="2">
-        <v>47.55</v>
+        <v>48.2</v>
       </c>
       <c r="K15" s="2">
-        <v>2187</v>
+        <v>2217</v>
       </c>
       <c r="N15" s="2" t="s">
         <v>16</v>
@@ -1136,19 +1136,19 @@
         <v>5962</v>
       </c>
       <c r="G16" s="2">
-        <v>5648</v>
+        <v>5542</v>
       </c>
       <c r="H16" s="2">
-        <v>-314</v>
+        <v>-420</v>
       </c>
       <c r="I16" s="3">
-        <v>-5.2999999999999999E-2</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="J16" s="2">
-        <v>158.5</v>
+        <v>155.5</v>
       </c>
       <c r="K16" s="2">
-        <v>5706</v>
+        <v>5598</v>
       </c>
       <c r="N16" s="2" t="s">
         <v>16</v>
@@ -1174,19 +1174,19 @@
         <v>6675</v>
       </c>
       <c r="G17" s="2">
-        <v>7373</v>
+        <v>7346</v>
       </c>
       <c r="H17" s="2">
-        <v>698</v>
+        <v>671</v>
       </c>
       <c r="I17" s="3">
-        <v>0.105</v>
+        <v>0.10100000000000001</v>
       </c>
       <c r="J17" s="2">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="K17" s="2">
-        <v>7434</v>
+        <v>7407</v>
       </c>
       <c r="N17" s="2" t="s">
         <v>16</v>
@@ -1203,28 +1203,28 @@
         <v>15</v>
       </c>
       <c r="D18" s="2">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E18" s="2">
-        <v>146.5</v>
+        <v>144.72999999999999</v>
       </c>
       <c r="F18" s="2">
-        <v>2346</v>
+        <v>3187</v>
       </c>
       <c r="G18" s="2">
-        <v>2206</v>
+        <v>3087</v>
       </c>
       <c r="H18" s="2">
-        <v>-140</v>
+        <v>-100</v>
       </c>
       <c r="I18" s="3">
-        <v>-0.06</v>
+        <v>-3.1E-2</v>
       </c>
       <c r="J18" s="2">
-        <v>139.5</v>
+        <v>142.5</v>
       </c>
       <c r="K18" s="2">
-        <v>2232</v>
+        <v>3135</v>
       </c>
       <c r="N18" s="2" t="s">
         <v>16</v>
@@ -1244,25 +1244,25 @@
         <v>13</v>
       </c>
       <c r="E19" s="2">
-        <v>240.46</v>
+        <v>212.92</v>
       </c>
       <c r="F19" s="2">
-        <v>3128</v>
+        <v>2770</v>
       </c>
       <c r="G19" s="2">
-        <v>2741</v>
+        <v>2482</v>
       </c>
       <c r="H19" s="2">
-        <v>-387</v>
+        <v>-288</v>
       </c>
       <c r="I19" s="3">
-        <v>-0.124</v>
+        <v>-0.104</v>
       </c>
       <c r="J19" s="2">
-        <v>213</v>
+        <v>193</v>
       </c>
       <c r="K19" s="2">
-        <v>2769</v>
+        <v>2509</v>
       </c>
       <c r="N19" s="2" t="s">
         <v>16</v>
@@ -1288,19 +1288,19 @@
         <v>3182</v>
       </c>
       <c r="G20" s="2">
-        <v>3058</v>
+        <v>3008</v>
       </c>
       <c r="H20" s="2">
-        <v>-124</v>
+        <v>-174</v>
       </c>
       <c r="I20" s="3">
-        <v>-3.9E-2</v>
+        <v>-5.5E-2</v>
       </c>
       <c r="J20" s="2">
-        <v>123.5</v>
+        <v>121.5</v>
       </c>
       <c r="K20" s="2">
-        <v>3088</v>
+        <v>3038</v>
       </c>
       <c r="N20" s="2" t="s">
         <v>16</v>
@@ -1311,19 +1311,19 @@
         <v>35</v>
       </c>
       <c r="F21" s="2">
-        <v>509254</v>
+        <v>510995</v>
       </c>
       <c r="G21" s="2">
-        <v>558559</v>
+        <v>564807</v>
       </c>
       <c r="H21" s="2">
-        <v>49305</v>
+        <v>53812</v>
       </c>
       <c r="I21" s="3">
-        <v>9.7000000000000003E-2</v>
+        <v>0.105</v>
       </c>
       <c r="K21" s="2">
-        <v>561619</v>
+        <v>567931</v>
       </c>
       <c r="N21" s="2" t="s">
         <v>16</v>

</xml_diff>